<commit_message>
added functions to process file data and copyText
getTotalRows, getTotalAmount, getInvoices, copytText button
</commit_message>
<xml_diff>
--- a/rts_test.xlsx
+++ b/rts_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\Documents\GitHub\RTS_Upload_Manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4259F5CC-D8F5-4479-B2D2-2F906B42B7F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122F8BD1-F027-484F-B052-F20E3E013BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{99D9E3DC-BC6B-45E7-A168-856168D82992}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
   <si>
     <t>ClientNo</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>COMPANY 15</t>
+  </si>
+  <si>
+    <t>InvAmt</t>
   </si>
 </sst>
 </file>
@@ -681,9 +684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7978454E-2600-4718-9BA0-D42F0317F5EC}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -715,7 +716,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
worked on verifying invoices
</commit_message>
<xml_diff>
--- a/rts_test.xlsx
+++ b/rts_test.xlsx
@@ -865,8 +865,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003820C8D89FBC5A498EDCF2655CC36A3C" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e57a22a07fc9c6068ef62b60b9a1381">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ca98ee16-d931-4edf-a6e2-f59632da0e93" xmlns:ns3="e0fc93d9-99b7-46c9-8e7b-843b4478b5a8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="45d5d35344668c8a3e510337905a14ef" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003820C8D89FBC5A498EDCF2655CC36A3C" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2f4afb9c099ce9358e40b68f74e5b75">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ca98ee16-d931-4edf-a6e2-f59632da0e93" xmlns:ns3="e0fc93d9-99b7-46c9-8e7b-843b4478b5a8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="559ef355ff75f9112597f82acb83b0dd" ns2:_="" ns3:_="">
     <xsd:import namespace="ca98ee16-d931-4edf-a6e2-f59632da0e93"/>
     <xsd:import namespace="e0fc93d9-99b7-46c9-8e7b-843b4478b5a8"/>
     <xsd:element name="properties">
@@ -888,6 +888,8 @@
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -956,6 +958,13 @@
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="3acfe6f2-be93-4c7f-9421-ad7279aac1a0" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e0fc93d9-99b7-46c9-8e7b-843b4478b5a8" elementFormDefault="qualified">
@@ -986,6 +995,17 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="23" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{d6196849-25f3-4b2d-9ad6-21140e912db7}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="e0fc93d9-99b7-46c9-8e7b-843b4478b5a8">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -1098,12 +1118,17 @@
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ca98ee16-d931-4edf-a6e2-f59632da0e93">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="e0fc93d9-99b7-46c9-8e7b-843b4478b5a8" xsi:nil="true"/>
+  </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{202EAAF0-6FCC-4D20-ADFA-29F71E3F403C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{600FA1CA-9E11-42A4-9E3D-EF7AA892306A}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>